<commit_message>
updated dan contact info
</commit_message>
<xml_diff>
--- a/_data/faculty.xlsx
+++ b/_data/faculty.xlsx
@@ -133,9 +133,6 @@
     <t>Assistant Professor</t>
   </si>
   <si>
-    <t>daniel.aukes@asu.edu</t>
-  </si>
-  <si>
     <t>POLY</t>
   </si>
   <si>
@@ -785,6 +782,9 @@
   </si>
   <si>
     <t>Gil</t>
+  </si>
+  <si>
+    <t>danaukes@asu.edu</t>
   </si>
 </sst>
 </file>
@@ -1627,7 +1627,7 @@
   <dimension ref="A1:N25"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+      <selection activeCell="E4" sqref="E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1781,43 +1781,43 @@
       <c r="D4" t="s">
         <v>38</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="1" t="s">
+        <v>256</v>
+      </c>
+      <c r="F4" t="s">
         <v>39</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>39</v>
+      </c>
+      <c r="H4" t="s">
         <v>40</v>
       </c>
-      <c r="G4" t="s">
-        <v>40</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>41</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>42</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>43</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>44</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>45</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>46</v>
-      </c>
-      <c r="N4" t="s">
-        <v>47</v>
       </c>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" t="s">
         <v>48</v>
-      </c>
-      <c r="B5" t="s">
-        <v>49</v>
       </c>
       <c r="C5" t="str">
         <f t="shared" si="0"/>
@@ -1827,42 +1827,42 @@
         <v>38</v>
       </c>
       <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
+        <v>39</v>
+      </c>
+      <c r="G5" t="s">
+        <v>39</v>
+      </c>
+      <c r="H5" t="s">
         <v>50</v>
       </c>
-      <c r="F5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G5" t="s">
-        <v>40</v>
-      </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>51</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>52</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>53</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>54</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>55</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>56</v>
-      </c>
-      <c r="N5" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B6" t="s">
         <v>58</v>
-      </c>
-      <c r="B6" t="s">
-        <v>59</v>
       </c>
       <c r="C6" t="str">
         <f t="shared" si="0"/>
@@ -1872,7 +1872,7 @@
         <v>16</v>
       </c>
       <c r="E6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="F6" t="s">
         <v>18</v>
@@ -1881,33 +1881,33 @@
         <v>18</v>
       </c>
       <c r="H6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I6" t="s">
         <v>61</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>62</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>63</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>64</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>65</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>66</v>
-      </c>
-      <c r="N6" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
+        <v>67</v>
+      </c>
+      <c r="B7" t="s">
         <v>68</v>
-      </c>
-      <c r="B7" t="s">
-        <v>69</v>
       </c>
       <c r="C7" t="str">
         <f t="shared" si="0"/>
@@ -1917,42 +1917,42 @@
         <v>38</v>
       </c>
       <c r="E7" t="s">
+        <v>69</v>
+      </c>
+      <c r="F7" t="s">
         <v>70</v>
       </c>
-      <c r="F7" t="s">
+      <c r="G7" t="s">
+        <v>70</v>
+      </c>
+      <c r="H7" t="s">
         <v>71</v>
       </c>
-      <c r="G7" t="s">
-        <v>71</v>
-      </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>72</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>73</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>74</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>75</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>76</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>77</v>
-      </c>
-      <c r="N7" t="s">
-        <v>78</v>
       </c>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>78</v>
+      </c>
+      <c r="B8" t="s">
         <v>79</v>
-      </c>
-      <c r="B8" t="s">
-        <v>80</v>
       </c>
       <c r="C8" t="str">
         <f t="shared" si="0"/>
@@ -1962,7 +1962,7 @@
         <v>38</v>
       </c>
       <c r="E8" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="F8" t="s">
         <v>18</v>
@@ -1971,33 +1971,33 @@
         <v>18</v>
       </c>
       <c r="H8" t="s">
+        <v>81</v>
+      </c>
+      <c r="I8" t="s">
         <v>82</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>83</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>84</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>85</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>86</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>87</v>
-      </c>
-      <c r="N8" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>88</v>
+      </c>
+      <c r="B9" t="s">
         <v>89</v>
-      </c>
-      <c r="B9" t="s">
-        <v>90</v>
       </c>
       <c r="C9" t="str">
         <f t="shared" si="0"/>
@@ -2007,42 +2007,42 @@
         <v>38</v>
       </c>
       <c r="E9" t="s">
+        <v>90</v>
+      </c>
+      <c r="F9" t="s">
+        <v>70</v>
+      </c>
+      <c r="G9" t="s">
+        <v>70</v>
+      </c>
+      <c r="H9" t="s">
         <v>91</v>
       </c>
-      <c r="F9" t="s">
-        <v>71</v>
-      </c>
-      <c r="G9" t="s">
-        <v>71</v>
-      </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>92</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>93</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>94</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>95</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>96</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>97</v>
-      </c>
-      <c r="N9" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
+        <v>98</v>
+      </c>
+      <c r="B10" t="s">
         <v>99</v>
-      </c>
-      <c r="B10" t="s">
-        <v>100</v>
       </c>
       <c r="C10" t="str">
         <f t="shared" si="0"/>
@@ -2052,84 +2052,84 @@
         <v>16</v>
       </c>
       <c r="E10" t="s">
+        <v>100</v>
+      </c>
+      <c r="F10" t="s">
+        <v>70</v>
+      </c>
+      <c r="G10" t="s">
+        <v>70</v>
+      </c>
+      <c r="H10" t="s">
         <v>101</v>
       </c>
-      <c r="F10" t="s">
-        <v>71</v>
-      </c>
-      <c r="G10" t="s">
-        <v>71</v>
-      </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>102</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>103</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>104</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>105</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>106</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>107</v>
-      </c>
-      <c r="N10" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
+        <v>108</v>
+      </c>
+      <c r="B11" t="s">
         <v>109</v>
-      </c>
-      <c r="B11" t="s">
-        <v>110</v>
       </c>
       <c r="C11" t="str">
         <f t="shared" si="0"/>
         <v>Pauline Davies</v>
       </c>
       <c r="D11" t="s">
+        <v>110</v>
+      </c>
+      <c r="E11" t="s">
         <v>111</v>
       </c>
-      <c r="E11" t="s">
+      <c r="F11" t="s">
         <v>112</v>
       </c>
-      <c r="F11" t="s">
+      <c r="G11" t="s">
         <v>113</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>114</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>115</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>116</v>
       </c>
-      <c r="J11" t="s">
+      <c r="L11" t="s">
         <v>117</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>118</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>119</v>
-      </c>
-      <c r="N11" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
+        <v>120</v>
+      </c>
+      <c r="B12" t="s">
         <v>121</v>
-      </c>
-      <c r="B12" t="s">
-        <v>122</v>
       </c>
       <c r="C12" t="str">
         <f t="shared" si="0"/>
@@ -2139,52 +2139,52 @@
         <v>16</v>
       </c>
       <c r="E12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" t="s">
+        <v>70</v>
+      </c>
+      <c r="G12" t="s">
+        <v>70</v>
+      </c>
+      <c r="H12" t="s">
         <v>123</v>
       </c>
-      <c r="F12" t="s">
-        <v>71</v>
-      </c>
-      <c r="G12" t="s">
-        <v>71</v>
-      </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>124</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>125</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>126</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>127</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>128</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>129</v>
-      </c>
-      <c r="N12" t="s">
-        <v>130</v>
       </c>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>130</v>
+      </c>
+      <c r="B13" t="s">
         <v>131</v>
-      </c>
-      <c r="B13" t="s">
-        <v>132</v>
       </c>
       <c r="C13" t="str">
         <f t="shared" si="0"/>
         <v>Subbarao Kambhampati</v>
       </c>
       <c r="D13" t="s">
+        <v>132</v>
+      </c>
+      <c r="E13" t="s">
         <v>133</v>
-      </c>
-      <c r="E13" t="s">
-        <v>134</v>
       </c>
       <c r="F13" t="s">
         <v>18</v>
@@ -2193,30 +2193,30 @@
         <v>18</v>
       </c>
       <c r="H13" t="s">
+        <v>134</v>
+      </c>
+      <c r="J13" t="s">
         <v>135</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>136</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
+        <v>134</v>
+      </c>
+      <c r="M13" t="s">
         <v>137</v>
       </c>
-      <c r="L13" t="s">
-        <v>135</v>
-      </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>138</v>
-      </c>
-      <c r="N13" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
+        <v>139</v>
+      </c>
+      <c r="B14" t="s">
         <v>140</v>
-      </c>
-      <c r="B14" t="s">
-        <v>141</v>
       </c>
       <c r="C14" t="str">
         <f t="shared" si="0"/>
@@ -2226,7 +2226,7 @@
         <v>38</v>
       </c>
       <c r="E14" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="F14" t="s">
         <v>18</v>
@@ -2235,88 +2235,88 @@
         <v>18</v>
       </c>
       <c r="H14" t="s">
+        <v>142</v>
+      </c>
+      <c r="I14" t="s">
         <v>143</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>144</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>145</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>146</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>147</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>148</v>
-      </c>
-      <c r="N14" t="s">
-        <v>149</v>
       </c>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
+        <v>149</v>
+      </c>
+      <c r="B15" t="s">
         <v>150</v>
-      </c>
-      <c r="B15" t="s">
-        <v>151</v>
       </c>
       <c r="C15" t="str">
         <f t="shared" si="0"/>
         <v>Thomas Sugar</v>
       </c>
       <c r="D15" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E15" t="s">
+        <v>151</v>
+      </c>
+      <c r="F15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G15" t="s">
+        <v>39</v>
+      </c>
+      <c r="H15" t="s">
         <v>152</v>
       </c>
-      <c r="F15" t="s">
-        <v>40</v>
-      </c>
-      <c r="G15" t="s">
-        <v>40</v>
-      </c>
-      <c r="H15" t="s">
+      <c r="I15" t="s">
         <v>153</v>
       </c>
-      <c r="I15" t="s">
+      <c r="J15" t="s">
         <v>154</v>
       </c>
-      <c r="J15" t="s">
+      <c r="K15" t="s">
         <v>155</v>
       </c>
-      <c r="K15" t="s">
+      <c r="L15" t="s">
         <v>156</v>
       </c>
-      <c r="L15" t="s">
+      <c r="M15" t="s">
         <v>157</v>
       </c>
-      <c r="M15" t="s">
+      <c r="N15" t="s">
         <v>158</v>
-      </c>
-      <c r="N15" t="s">
-        <v>159</v>
       </c>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
+        <v>159</v>
+      </c>
+      <c r="B16" t="s">
         <v>160</v>
-      </c>
-      <c r="B16" t="s">
-        <v>161</v>
       </c>
       <c r="C16" t="str">
         <f t="shared" si="0"/>
         <v>Thurmon Lockhart</v>
       </c>
       <c r="D16" t="s">
+        <v>161</v>
+      </c>
+      <c r="E16" t="s">
         <v>162</v>
-      </c>
-      <c r="E16" t="s">
-        <v>163</v>
       </c>
       <c r="F16" t="s">
         <v>28</v>
@@ -2325,33 +2325,33 @@
         <v>28</v>
       </c>
       <c r="H16" t="s">
+        <v>163</v>
+      </c>
+      <c r="I16" t="s">
         <v>164</v>
       </c>
-      <c r="I16" t="s">
+      <c r="J16" t="s">
         <v>165</v>
       </c>
-      <c r="J16" t="s">
+      <c r="K16" t="s">
         <v>166</v>
       </c>
-      <c r="K16" t="s">
+      <c r="L16" t="s">
         <v>167</v>
       </c>
-      <c r="L16" t="s">
+      <c r="M16" t="s">
         <v>168</v>
       </c>
-      <c r="M16" t="s">
+      <c r="N16" t="s">
         <v>169</v>
-      </c>
-      <c r="N16" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
+        <v>170</v>
+      </c>
+      <c r="B17" t="s">
         <v>171</v>
-      </c>
-      <c r="B17" t="s">
-        <v>172</v>
       </c>
       <c r="C17" t="str">
         <f t="shared" si="0"/>
@@ -2361,42 +2361,42 @@
         <v>38</v>
       </c>
       <c r="E17" t="s">
+        <v>172</v>
+      </c>
+      <c r="F17" t="s">
+        <v>39</v>
+      </c>
+      <c r="G17" t="s">
+        <v>39</v>
+      </c>
+      <c r="H17" t="s">
         <v>173</v>
       </c>
-      <c r="F17" t="s">
-        <v>40</v>
-      </c>
-      <c r="G17" t="s">
-        <v>40</v>
-      </c>
-      <c r="H17" t="s">
+      <c r="I17" t="s">
         <v>174</v>
       </c>
-      <c r="I17" t="s">
+      <c r="J17" t="s">
         <v>175</v>
       </c>
-      <c r="J17" t="s">
+      <c r="K17" t="s">
         <v>176</v>
       </c>
-      <c r="K17" t="s">
+      <c r="L17" t="s">
         <v>177</v>
       </c>
-      <c r="L17" t="s">
+      <c r="M17" t="s">
         <v>178</v>
       </c>
-      <c r="M17" t="s">
+      <c r="N17" t="s">
         <v>179</v>
-      </c>
-      <c r="N17" t="s">
-        <v>180</v>
       </c>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
+        <v>180</v>
+      </c>
+      <c r="B18" t="s">
         <v>181</v>
-      </c>
-      <c r="B18" t="s">
-        <v>182</v>
       </c>
       <c r="C18" t="str">
         <f t="shared" si="0"/>
@@ -2406,7 +2406,7 @@
         <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F18" t="s">
         <v>18</v>
@@ -2415,33 +2415,33 @@
         <v>18</v>
       </c>
       <c r="H18" t="s">
+        <v>183</v>
+      </c>
+      <c r="I18" t="s">
         <v>184</v>
       </c>
-      <c r="I18" t="s">
+      <c r="J18" t="s">
         <v>185</v>
       </c>
-      <c r="J18" t="s">
+      <c r="K18" t="s">
         <v>186</v>
       </c>
-      <c r="K18" t="s">
+      <c r="L18" t="s">
         <v>187</v>
       </c>
-      <c r="L18" t="s">
+      <c r="M18" t="s">
         <v>188</v>
       </c>
-      <c r="M18" t="s">
+      <c r="N18" t="s">
         <v>189</v>
-      </c>
-      <c r="N18" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
+        <v>190</v>
+      </c>
+      <c r="B19" t="s">
         <v>191</v>
-      </c>
-      <c r="B19" t="s">
-        <v>192</v>
       </c>
       <c r="C19" t="str">
         <f t="shared" si="0"/>
@@ -2451,52 +2451,52 @@
         <v>38</v>
       </c>
       <c r="E19" t="s">
+        <v>192</v>
+      </c>
+      <c r="F19" t="s">
+        <v>70</v>
+      </c>
+      <c r="G19" t="s">
+        <v>70</v>
+      </c>
+      <c r="H19" t="s">
         <v>193</v>
       </c>
-      <c r="F19" t="s">
-        <v>71</v>
-      </c>
-      <c r="G19" t="s">
-        <v>71</v>
-      </c>
-      <c r="H19" t="s">
+      <c r="I19" t="s">
         <v>194</v>
       </c>
-      <c r="I19" t="s">
+      <c r="J19" t="s">
         <v>195</v>
       </c>
-      <c r="J19" t="s">
+      <c r="K19" t="s">
         <v>196</v>
       </c>
-      <c r="K19" t="s">
+      <c r="L19" t="s">
         <v>197</v>
       </c>
-      <c r="L19" t="s">
+      <c r="M19" t="s">
         <v>198</v>
       </c>
-      <c r="M19" t="s">
+      <c r="N19" t="s">
         <v>199</v>
-      </c>
-      <c r="N19" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B20" t="s">
         <v>201</v>
-      </c>
-      <c r="B20" t="s">
-        <v>202</v>
       </c>
       <c r="C20" t="str">
         <f t="shared" si="0"/>
         <v>Yinong Chen</v>
       </c>
       <c r="D20" t="s">
+        <v>202</v>
+      </c>
+      <c r="E20" t="s">
         <v>203</v>
-      </c>
-      <c r="E20" t="s">
-        <v>204</v>
       </c>
       <c r="F20" t="s">
         <v>18</v>
@@ -2505,33 +2505,33 @@
         <v>18</v>
       </c>
       <c r="H20" t="s">
+        <v>204</v>
+      </c>
+      <c r="I20" t="s">
         <v>205</v>
       </c>
-      <c r="I20" t="s">
+      <c r="J20" t="s">
         <v>206</v>
       </c>
-      <c r="J20" t="s">
+      <c r="K20" t="s">
         <v>207</v>
       </c>
-      <c r="K20" t="s">
+      <c r="L20" t="s">
         <v>208</v>
       </c>
-      <c r="L20" t="s">
+      <c r="M20" t="s">
         <v>209</v>
       </c>
-      <c r="M20" t="s">
+      <c r="N20" t="s">
         <v>210</v>
-      </c>
-      <c r="N20" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B21" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C21" t="str">
         <f t="shared" si="0"/>
@@ -2541,7 +2541,7 @@
         <v>38</v>
       </c>
       <c r="E21" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="F21" t="s">
         <v>18</v>
@@ -2550,33 +2550,33 @@
         <v>18</v>
       </c>
       <c r="H21" t="s">
+        <v>213</v>
+      </c>
+      <c r="I21" t="s">
         <v>214</v>
       </c>
-      <c r="I21" t="s">
+      <c r="J21" t="s">
         <v>215</v>
       </c>
-      <c r="J21" t="s">
+      <c r="K21" t="s">
         <v>216</v>
       </c>
-      <c r="K21" t="s">
+      <c r="L21" t="s">
         <v>217</v>
       </c>
-      <c r="L21" t="s">
+      <c r="M21" t="s">
         <v>218</v>
       </c>
-      <c r="M21" t="s">
+      <c r="N21" t="s">
         <v>219</v>
-      </c>
-      <c r="N21" t="s">
-        <v>220</v>
       </c>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
+        <v>220</v>
+      </c>
+      <c r="B22" t="s">
         <v>221</v>
-      </c>
-      <c r="B22" t="s">
-        <v>222</v>
       </c>
       <c r="C22" t="str">
         <f t="shared" si="0"/>
@@ -2586,7 +2586,7 @@
         <v>38</v>
       </c>
       <c r="E22" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="F22" t="s">
         <v>18</v>
@@ -2595,33 +2595,33 @@
         <v>18</v>
       </c>
       <c r="H22" t="s">
+        <v>223</v>
+      </c>
+      <c r="I22" t="s">
         <v>224</v>
       </c>
-      <c r="I22" t="s">
+      <c r="J22" t="s">
         <v>225</v>
       </c>
-      <c r="J22" t="s">
+      <c r="K22" t="s">
         <v>226</v>
       </c>
-      <c r="K22" t="s">
+      <c r="L22" t="s">
         <v>227</v>
       </c>
-      <c r="L22" t="s">
+      <c r="M22" t="s">
         <v>228</v>
       </c>
-      <c r="M22" t="s">
+      <c r="N22" t="s">
         <v>229</v>
-      </c>
-      <c r="N22" t="s">
-        <v>230</v>
       </c>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A23" t="s">
+        <v>230</v>
+      </c>
+      <c r="B23" t="s">
         <v>231</v>
-      </c>
-      <c r="B23" t="s">
-        <v>232</v>
       </c>
       <c r="C23" t="str">
         <f t="shared" si="0"/>
@@ -2631,87 +2631,87 @@
         <v>38</v>
       </c>
       <c r="E23" t="s">
+        <v>232</v>
+      </c>
+      <c r="F23" t="s">
+        <v>70</v>
+      </c>
+      <c r="G23" t="s">
+        <v>70</v>
+      </c>
+      <c r="H23" t="s">
         <v>233</v>
       </c>
-      <c r="F23" t="s">
-        <v>71</v>
-      </c>
-      <c r="G23" t="s">
-        <v>71</v>
-      </c>
-      <c r="H23" t="s">
+      <c r="I23" t="s">
         <v>234</v>
       </c>
-      <c r="I23" t="s">
+      <c r="J23" t="s">
         <v>235</v>
       </c>
-      <c r="J23" t="s">
+      <c r="K23" t="s">
         <v>236</v>
       </c>
-      <c r="K23" t="s">
+      <c r="L23" t="s">
         <v>237</v>
       </c>
-      <c r="L23" t="s">
+      <c r="M23" t="s">
         <v>238</v>
       </c>
-      <c r="M23" t="s">
+      <c r="N23" t="s">
         <v>239</v>
-      </c>
-      <c r="N23" t="s">
-        <v>240</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" t="s">
         <v>241</v>
-      </c>
-      <c r="B24" t="s">
-        <v>242</v>
       </c>
       <c r="C24" t="str">
         <f t="shared" si="0"/>
         <v>Lina Karam</v>
       </c>
       <c r="D24" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E24" t="s">
+        <v>242</v>
+      </c>
+      <c r="F24" t="s">
         <v>243</v>
       </c>
-      <c r="F24" t="s">
+      <c r="G24" t="s">
+        <v>243</v>
+      </c>
+      <c r="H24" t="s">
         <v>244</v>
       </c>
-      <c r="G24" t="s">
-        <v>244</v>
-      </c>
-      <c r="H24" t="s">
+      <c r="I24" t="s">
         <v>245</v>
       </c>
-      <c r="I24" t="s">
+      <c r="J24" t="s">
         <v>246</v>
       </c>
-      <c r="J24" t="s">
+      <c r="K24" t="s">
         <v>247</v>
       </c>
-      <c r="K24" t="s">
+      <c r="L24" t="s">
         <v>248</v>
       </c>
-      <c r="L24" t="s">
+      <c r="M24" t="s">
         <v>249</v>
       </c>
-      <c r="M24" t="s">
+      <c r="N24" t="s">
         <v>250</v>
-      </c>
-      <c r="N24" t="s">
-        <v>251</v>
       </c>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B25" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="C25" t="str">
         <f t="shared" si="0"/>
@@ -2721,7 +2721,7 @@
         <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="F25" t="s">
         <v>18</v>
@@ -2730,16 +2730,17 @@
         <v>18</v>
       </c>
       <c r="J25" t="s">
+        <v>253</v>
+      </c>
+      <c r="K25" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>255</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E25" r:id="rId1"/>
     <hyperlink ref="K25" r:id="rId2"/>
+    <hyperlink ref="E4" r:id="rId3"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
updates to robotics website
</commit_message>
<xml_diff>
--- a/_data/faculty.xlsx
+++ b/_data/faculty.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\website_asurobotics\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2CF20ABB-F96C-449A-A1AD-8694A293C490}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{38C476B6-2AFB-435E-A004-88E1F36144B3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1950" yWindow="1950" windowWidth="28800" windowHeight="15555" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="5976" windowWidth="34560" windowHeight="18648" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="faculty" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="262">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="343" uniqueCount="273">
   <si>
     <t>first_name</t>
   </si>
@@ -165,9 +165,6 @@
     <t>The lab's focus is to develop new tools for designing robots by pairing emerging fabrication techniques and new materials with analytical and simulation-based methods for understanding the behavior of these complex systems</t>
   </si>
   <si>
-    <t>Aukes_Daniel_1208_w.jpg</t>
-  </si>
-  <si>
     <t>DSC_0006.JPG</t>
   </si>
   <si>
@@ -814,13 +811,49 @@
   </si>
   <si>
     <t>mcdaniel.jpg</t>
+  </si>
+  <si>
+    <t>Ayan</t>
+  </si>
+  <si>
+    <t>Malik</t>
+  </si>
+  <si>
+    <t>ayan.mallik@asu.edu</t>
+  </si>
+  <si>
+    <t> Working on the design, modelling, control and optimization of power electronic converters, characterizations and applications of wide bandgap (WBG) semiconductors, highly efficient &amp; high-power density solutions for power conversions in the applications of more-electric-aircrafts, electric vehicles, wireless charging and data centers.</t>
+  </si>
+  <si>
+    <t>Design,Controls</t>
+  </si>
+  <si>
+    <t>Laboratory for Power Electronics Systems (LPES)</t>
+  </si>
+  <si>
+    <t>The objective of LPES is to perform multidimensional co-design and optimization of power electronic systems for a variety of applications such as: transportation electrification, data centers etc. We are pursuing a multi-disciplinary research agenda merging thermal and reliability constraints with power electronics design for the research problems that are attempting to achieve challenging targets for multiple performance metrics (such as: power density, efficiency, and reliability, etc).</t>
+  </si>
+  <si>
+    <t>malik.jpg</t>
+  </si>
+  <si>
+    <t>mcdaniel_lab.jpg</t>
+  </si>
+  <si>
+    <t>sgil_headshot.jpg</t>
+  </si>
+  <si>
+    <t>Daniel-Aukes.jpg</t>
+  </si>
+  <si>
+    <t>gil_lab.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="22" x14ac:knownFonts="1">
+  <fonts count="23" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -985,6 +1018,12 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF2A2A2A"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="33">
     <fill>
@@ -1328,7 +1367,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -1340,6 +1379,7 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="43">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1720,30 +1760,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:N26"/>
+  <dimension ref="A1:N27"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="L3" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L15" sqref="L15"/>
+    <sheetView tabSelected="1" topLeftCell="I9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="13.8" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="12.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.5546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="12" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="30.140625" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="23.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="38.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="30.109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="23.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="38.33203125" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.88671875" style="1" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="75" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="11" width="40.7109375" style="1" customWidth="1"/>
-    <col min="12" max="12" width="80.5703125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="33.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="52.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="16384" width="9.140625" style="1"/>
+    <col min="9" max="11" width="40.6640625" style="1" customWidth="1"/>
+    <col min="12" max="12" width="80.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="33.5546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="52.88671875" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="9.109375" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1787,7 +1827,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="2" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>36</v>
       </c>
@@ -1795,14 +1835,14 @@
         <v>37</v>
       </c>
       <c r="C2" s="1" t="str">
-        <f t="shared" ref="C2:C26" si="0">A2&amp;" "&amp;B2</f>
+        <f t="shared" ref="C2:C27" si="0">A2&amp;" "&amp;B2</f>
         <v>Daniel Aukes</v>
       </c>
       <c r="D2" s="1" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>39</v>
@@ -1826,18 +1866,18 @@
         <v>44</v>
       </c>
       <c r="M2" s="1" t="s">
+        <v>271</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="N2" s="1" t="s">
-        <v>46</v>
-      </c>
     </row>
-    <row r="3" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>78</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>79</v>
       </c>
       <c r="C3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1847,7 +1887,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>18</v>
@@ -1856,33 +1896,33 @@
         <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>80</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>84</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>87</v>
-      </c>
     </row>
-    <row r="4" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>110</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>111</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1892,37 +1932,37 @@
         <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>112</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>115</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="3" t="s">
         <v>116</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>118</v>
       </c>
-      <c r="N4" s="1" t="s">
-        <v>119</v>
-      </c>
     </row>
-    <row r="5" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>25</v>
       </c>
@@ -1967,22 +2007,22 @@
         <v>35</v>
       </c>
     </row>
-    <row r="6" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>190</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>191</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Yinong Chen</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>191</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>192</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>193</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
@@ -1991,33 +2031,33 @@
         <v>18</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>193</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>196</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="3" t="s">
         <v>197</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="1" t="s">
         <v>198</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>199</v>
       </c>
-      <c r="N6" s="1" t="s">
-        <v>200</v>
-      </c>
     </row>
-    <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>48</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2027,7 +2067,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>39</v>
@@ -2036,75 +2076,75 @@
         <v>39</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="N7" s="1" t="s">
-        <v>56</v>
-      </c>
     </row>
-    <row r="8" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>98</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>99</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Pauline Davies</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>103</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="3" t="s">
         <v>106</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="1" t="s">
         <v>107</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="N8" s="1" t="s">
-        <v>109</v>
-      </c>
     </row>
-    <row r="9" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>58</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2114,7 +2154,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>18</v>
@@ -2123,33 +2163,33 @@
         <v>18</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="N9" s="1" t="s">
-        <v>66</v>
-      </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
       <c r="A10" s="1" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2159,7 +2199,7 @@
         <v>38</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>18</v>
@@ -2168,28 +2208,34 @@
         <v>18</v>
       </c>
       <c r="J10" s="1" t="s">
+        <v>241</v>
+      </c>
+      <c r="K10" s="2" t="s">
         <v>242</v>
       </c>
-      <c r="K10" s="2" t="s">
-        <v>243</v>
+      <c r="M10" s="1" t="s">
+        <v>270</v>
+      </c>
+      <c r="N10" s="1" t="s">
+        <v>272</v>
       </c>
     </row>
-    <row r="11" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A11" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>120</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>121</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Subbarao Kambhampati</v>
       </c>
       <c r="D11" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="E11" s="1" t="s">
         <v>122</v>
-      </c>
-      <c r="E11" s="1" t="s">
-        <v>123</v>
       </c>
       <c r="F11" s="1" t="s">
         <v>18</v>
@@ -2198,75 +2244,75 @@
         <v>18</v>
       </c>
       <c r="H11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="J11" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="M11" s="1" t="s">
         <v>126</v>
       </c>
-      <c r="L11" s="3" t="s">
-        <v>124</v>
-      </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="N11" s="1" t="s">
-        <v>128</v>
-      </c>
     </row>
-    <row r="12" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A12" s="1" t="s">
+        <v>228</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>229</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>230</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Lina Karam</v>
       </c>
       <c r="D12" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="F12" s="1" t="s">
         <v>231</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="G12" s="1" t="s">
+        <v>231</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="G12" s="1" t="s">
-        <v>232</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>235</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="3" t="s">
         <v>236</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="1" t="s">
         <v>237</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>238</v>
       </c>
-      <c r="N12" s="1" t="s">
-        <v>239</v>
-      </c>
     </row>
-    <row r="13" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A13" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>88</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>89</v>
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2276,52 +2322,52 @@
         <v>38</v>
       </c>
       <c r="E13" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="F13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G13" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H13" s="3" t="s">
         <v>90</v>
       </c>
-      <c r="F13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G13" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="I13" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="1" t="s">
         <v>95</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="N13" s="1" t="s">
-        <v>97</v>
-      </c>
     </row>
-    <row r="14" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A14" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Thurmon Lockhart</v>
       </c>
       <c r="D14" s="1" t="s">
+        <v>150</v>
+      </c>
+      <c r="E14" s="1" t="s">
         <v>151</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>152</v>
       </c>
       <c r="F14" s="1" t="s">
         <v>28</v>
@@ -2330,33 +2376,33 @@
         <v>28</v>
       </c>
       <c r="H14" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="I14" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>155</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="3" t="s">
         <v>156</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="1" t="s">
         <v>157</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>158</v>
       </c>
-      <c r="N14" s="1" t="s">
-        <v>159</v>
-      </c>
     </row>
-    <row r="15" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A15" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>68</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2366,42 +2412,42 @@
         <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="F15" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="1" t="s">
+      <c r="G15" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H15" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="I15" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>73</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="M15" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="N15" s="1" t="s">
-        <v>77</v>
-      </c>
     </row>
-    <row r="16" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A16" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>129</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>130</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2411,7 +2457,7 @@
         <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F16" s="1" t="s">
         <v>18</v>
@@ -2420,33 +2466,33 @@
         <v>18</v>
       </c>
       <c r="H16" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="I16" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>134</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="3" t="s">
         <v>135</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>137</v>
       </c>
-      <c r="N16" s="1" t="s">
-        <v>138</v>
-      </c>
     </row>
-    <row r="17" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A17" s="1" t="s">
+        <v>179</v>
+      </c>
+      <c r="B17" s="1" t="s">
         <v>180</v>
-      </c>
-      <c r="B17" s="1" t="s">
-        <v>181</v>
       </c>
       <c r="C17" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2456,37 +2502,37 @@
         <v>38</v>
       </c>
       <c r="E17" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="F17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G17" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H17" s="3" t="s">
         <v>182</v>
       </c>
-      <c r="F17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G17" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H17" s="3" t="s">
+      <c r="I17" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="J17" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="K17" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="L17" s="3" t="s">
         <v>186</v>
       </c>
-      <c r="L17" s="3" t="s">
+      <c r="M17" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="M17" s="1" t="s">
+      <c r="N17" s="1" t="s">
         <v>188</v>
       </c>
-      <c r="N17" s="1" t="s">
-        <v>189</v>
-      </c>
     </row>
-    <row r="18" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A18" s="1" t="s">
         <v>14</v>
       </c>
@@ -2528,12 +2574,12 @@
         <v>24</v>
       </c>
     </row>
-    <row r="19" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>210</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>211</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2543,7 +2589,7 @@
         <v>38</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>18</v>
@@ -2552,43 +2598,43 @@
         <v>18</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>212</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="M19" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>218</v>
       </c>
-      <c r="N19" s="1" t="s">
-        <v>219</v>
-      </c>
     </row>
-    <row r="20" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A20" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>139</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>140</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Thomas Sugar</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>39</v>
@@ -2597,33 +2643,33 @@
         <v>39</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="3" t="s">
         <v>145</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="N20" s="1" t="s">
-        <v>148</v>
-      </c>
     </row>
-    <row r="21" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A21" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>170</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>171</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2633,7 +2679,7 @@
         <v>38</v>
       </c>
       <c r="E21" s="1" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="F21" s="1" t="s">
         <v>18</v>
@@ -2642,33 +2688,33 @@
         <v>18</v>
       </c>
       <c r="H21" s="3" t="s">
+        <v>172</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="M21" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>178</v>
       </c>
-      <c r="N21" s="1" t="s">
-        <v>179</v>
-      </c>
     </row>
-    <row r="22" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A22" s="1" t="s">
+        <v>219</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>220</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>221</v>
       </c>
       <c r="C22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2678,42 +2724,42 @@
         <v>38</v>
       </c>
       <c r="E22" s="1" t="s">
+        <v>221</v>
+      </c>
+      <c r="F22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="G22" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>245</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="F22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="G22" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="H22" s="3" t="s">
-        <v>246</v>
-      </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="M22" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>227</v>
       </c>
-      <c r="N22" s="1" t="s">
-        <v>228</v>
-      </c>
     </row>
-    <row r="23" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:14" ht="27.6" x14ac:dyDescent="0.3">
       <c r="A23" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B23" s="1" t="s">
         <v>160</v>
-      </c>
-      <c r="B23" s="1" t="s">
-        <v>161</v>
       </c>
       <c r="C23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2723,7 +2769,7 @@
         <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>39</v>
@@ -2732,33 +2778,33 @@
         <v>39</v>
       </c>
       <c r="H23" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="3" t="s">
         <v>166</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="M23" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="N23" s="1" t="s">
-        <v>169</v>
-      </c>
     </row>
-    <row r="24" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:14" ht="41.4" x14ac:dyDescent="0.3">
       <c r="A24" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2768,7 +2814,7 @@
         <v>38</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>18</v>
@@ -2777,33 +2823,33 @@
         <v>18</v>
       </c>
       <c r="H24" s="3" t="s">
+        <v>202</v>
+      </c>
+      <c r="I24" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="I24" s="1" t="s">
+      <c r="J24" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>205</v>
       </c>
-      <c r="K24" s="1" t="s">
+      <c r="L24" s="3" t="s">
         <v>206</v>
       </c>
-      <c r="L24" s="3" t="s">
+      <c r="M24" s="1" t="s">
         <v>207</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="N24" s="1" t="s">
-        <v>209</v>
-      </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>246</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>247</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>248</v>
       </c>
       <c r="C25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2813,7 +2859,7 @@
         <v>16</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>39</v>
@@ -2822,33 +2868,33 @@
         <v>39</v>
       </c>
       <c r="H25" s="3" t="s">
+        <v>252</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>142</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="K25" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="L25" s="4" t="s">
+        <v>249</v>
+      </c>
+      <c r="M25" s="1" t="s">
+        <v>250</v>
+      </c>
+      <c r="N25" s="1" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" ht="55.2" x14ac:dyDescent="0.3">
+      <c r="A26" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="I25" s="1" t="s">
-        <v>143</v>
-      </c>
-      <c r="J25" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="K25" s="1" t="s">
-        <v>145</v>
-      </c>
-      <c r="L25" s="4" t="s">
-        <v>250</v>
-      </c>
-      <c r="M25" s="1" t="s">
-        <v>251</v>
-      </c>
-      <c r="N25" s="1" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="26" spans="1:14" ht="51" x14ac:dyDescent="0.25">
-      <c r="A26" s="1" t="s">
+      <c r="B26" s="1" t="s">
         <v>254</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>255</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2858,22 +2904,70 @@
         <v>38</v>
       </c>
       <c r="E26" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="F26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G26" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H26" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="H26" s="3" t="s">
+      <c r="I26" s="1" t="s">
         <v>257</v>
       </c>
-      <c r="I26" s="1" t="s">
+      <c r="J26" s="1" t="s">
         <v>258</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="3" t="s">
         <v>259</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="M26" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="M26" s="1" t="s">
+      <c r="N26" s="1" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" ht="69" x14ac:dyDescent="0.25">
+      <c r="A27" s="1" t="s">
         <v>261</v>
+      </c>
+      <c r="B27" s="1" t="s">
+        <v>262</v>
+      </c>
+      <c r="C27" s="1" t="str">
+        <f t="shared" si="0"/>
+        <v>Ayan Malik</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="E27" s="1" t="s">
+        <v>263</v>
+      </c>
+      <c r="F27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="H27" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="I27" s="5" t="s">
+        <v>265</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>266</v>
+      </c>
+      <c r="L27" s="3" t="s">
+        <v>267</v>
+      </c>
+      <c r="M27" s="1" t="s">
+        <v>268</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated pages a bit
</commit_message>
<xml_diff>
--- a/_data/faculty.xlsx
+++ b/_data/faculty.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\danaukes\websites\website_asurobotics\_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5A37B27E-2D78-434B-926C-8AE964EA09B7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C2C0C83-7204-4927-9BC5-4E6D01B340A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -167,9 +167,6 @@
     <t>The lab's focus is to develop new tools for designing robots by pairing emerging fabrication techniques and new materials with analytical and simulation-based methods for understanding the behavior of these complex systems</t>
   </si>
   <si>
-    <t>DSC_0006.JPG</t>
-  </si>
-  <si>
     <t>Erin</t>
   </si>
   <si>
@@ -827,7 +824,10 @@
     <t>mcdaniel_lab.jpg</t>
   </si>
   <si>
-    <t>Daniel-Aukes.jpg</t>
+    <t>Aukes-37.jpg</t>
+  </si>
+  <si>
+    <t>POLY-Dan-Aukes-2020-EG-5546a.png</t>
   </si>
 </sst>
 </file>
@@ -1743,8 +1743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:N26"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A10" sqref="A10:XFD10"/>
+    <sheetView tabSelected="1" topLeftCell="I1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="M2" sqref="M2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -1823,7 +1823,7 @@
         <v>38</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="F2" s="1" t="s">
         <v>39</v>
@@ -1850,15 +1850,15 @@
         <v>265</v>
       </c>
       <c r="N2" s="1" t="s">
-        <v>45</v>
+        <v>264</v>
       </c>
     </row>
     <row r="3" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="C3" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1868,7 +1868,7 @@
         <v>38</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="F3" s="1" t="s">
         <v>18</v>
@@ -1877,33 +1877,33 @@
         <v>18</v>
       </c>
       <c r="H3" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="I3" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="I3" s="1" t="s">
+      <c r="J3" s="1" t="s">
         <v>81</v>
       </c>
-      <c r="J3" s="1" t="s">
+      <c r="K3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="K3" s="1" t="s">
+      <c r="L3" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="L3" s="3" t="s">
+      <c r="M3" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="M3" s="1" t="s">
+      <c r="N3" s="1" t="s">
         <v>85</v>
-      </c>
-      <c r="N3" s="1" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>109</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>110</v>
       </c>
       <c r="C4" s="1" t="str">
         <f t="shared" si="0"/>
@@ -1913,34 +1913,34 @@
         <v>16</v>
       </c>
       <c r="E4" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H4" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="F4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G4" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="I4" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="I4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>113</v>
       </c>
-      <c r="J4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="K4" s="1" t="s">
+      <c r="L4" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="L4" s="3" t="s">
+      <c r="M4" s="1" t="s">
         <v>116</v>
       </c>
-      <c r="M4" s="1" t="s">
+      <c r="N4" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="5" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
@@ -1990,20 +1990,20 @@
     </row>
     <row r="6" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>189</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>190</v>
       </c>
       <c r="C6" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Yinong Chen</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>191</v>
-      </c>
-      <c r="E6" s="1" t="s">
-        <v>192</v>
       </c>
       <c r="F6" s="1" t="s">
         <v>18</v>
@@ -2012,33 +2012,33 @@
         <v>18</v>
       </c>
       <c r="H6" s="3" t="s">
+        <v>192</v>
+      </c>
+      <c r="I6" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="I6" s="1" t="s">
+      <c r="J6" s="1" t="s">
         <v>194</v>
       </c>
-      <c r="J6" s="1" t="s">
+      <c r="K6" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="K6" s="1" t="s">
+      <c r="L6" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="L6" s="3" t="s">
+      <c r="M6" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="M6" s="1" t="s">
+      <c r="N6" s="1" t="s">
         <v>198</v>
-      </c>
-      <c r="N6" s="1" t="s">
-        <v>199</v>
       </c>
     </row>
     <row r="7" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="B7" s="1" t="s">
         <v>46</v>
-      </c>
-      <c r="B7" s="1" t="s">
-        <v>47</v>
       </c>
       <c r="C7" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2048,7 +2048,7 @@
         <v>38</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F7" s="1" t="s">
         <v>39</v>
@@ -2057,75 +2057,75 @@
         <v>39</v>
       </c>
       <c r="H7" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="I7" s="1" t="s">
+      <c r="J7" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="J7" s="1" t="s">
+      <c r="K7" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="K7" s="1" t="s">
+      <c r="L7" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="L7" s="3" t="s">
+      <c r="M7" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="M7" s="1" t="s">
+      <c r="N7" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="N7" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="8" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B8" s="1" t="s">
         <v>97</v>
-      </c>
-      <c r="B8" s="1" t="s">
-        <v>98</v>
       </c>
       <c r="C8" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Pauline Davies</v>
       </c>
       <c r="D8" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>99</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="F8" s="1" t="s">
         <v>100</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="G8" s="1" t="s">
         <v>101</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="H8" s="3" t="s">
         <v>102</v>
       </c>
-      <c r="H8" s="3" t="s">
+      <c r="I8" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="J8" s="1" t="s">
         <v>104</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="L8" s="3" t="s">
         <v>105</v>
       </c>
-      <c r="L8" s="3" t="s">
+      <c r="M8" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="M8" s="1" t="s">
+      <c r="N8" s="1" t="s">
         <v>107</v>
-      </c>
-      <c r="N8" s="1" t="s">
-        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B9" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="B9" s="1" t="s">
-        <v>57</v>
       </c>
       <c r="C9" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2135,7 +2135,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="F9" s="1" t="s">
         <v>18</v>
@@ -2144,43 +2144,43 @@
         <v>18</v>
       </c>
       <c r="H9" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="I9" s="1" t="s">
         <v>59</v>
       </c>
-      <c r="I9" s="1" t="s">
+      <c r="J9" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="J9" s="1" t="s">
+      <c r="K9" s="1" t="s">
         <v>61</v>
       </c>
-      <c r="K9" s="1" t="s">
+      <c r="L9" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="L9" s="3" t="s">
+      <c r="M9" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="M9" s="1" t="s">
+      <c r="N9" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="N9" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="10" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B10" s="1" t="s">
         <v>119</v>
-      </c>
-      <c r="B10" s="1" t="s">
-        <v>120</v>
       </c>
       <c r="C10" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Subbarao Kambhampati</v>
       </c>
       <c r="D10" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="E10" s="1" t="s">
         <v>121</v>
-      </c>
-      <c r="E10" s="1" t="s">
-        <v>122</v>
       </c>
       <c r="F10" s="1" t="s">
         <v>18</v>
@@ -2189,75 +2189,75 @@
         <v>18</v>
       </c>
       <c r="H10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="J10" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="J10" s="1" t="s">
+      <c r="K10" s="1" t="s">
         <v>124</v>
       </c>
-      <c r="K10" s="1" t="s">
+      <c r="L10" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="M10" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="L10" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="M10" s="1" t="s">
+      <c r="N10" s="1" t="s">
         <v>126</v>
-      </c>
-      <c r="N10" s="1" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="11" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
+        <v>227</v>
+      </c>
+      <c r="B11" s="1" t="s">
         <v>228</v>
-      </c>
-      <c r="B11" s="1" t="s">
-        <v>229</v>
       </c>
       <c r="C11" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Lina Karam</v>
       </c>
       <c r="D11" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E11" s="1" t="s">
+        <v>229</v>
+      </c>
+      <c r="F11" s="1" t="s">
         <v>230</v>
       </c>
-      <c r="F11" s="1" t="s">
+      <c r="G11" s="1" t="s">
+        <v>230</v>
+      </c>
+      <c r="H11" s="3" t="s">
         <v>231</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>231</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="I11" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="I11" s="1" t="s">
+      <c r="J11" s="1" t="s">
         <v>233</v>
       </c>
-      <c r="J11" s="1" t="s">
+      <c r="K11" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="K11" s="1" t="s">
+      <c r="L11" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="L11" s="3" t="s">
+      <c r="M11" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="M11" s="1" t="s">
+      <c r="N11" s="1" t="s">
         <v>237</v>
-      </c>
-      <c r="N11" s="1" t="s">
-        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="B12" s="1" t="s">
         <v>87</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>88</v>
       </c>
       <c r="C12" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2267,52 +2267,52 @@
         <v>38</v>
       </c>
       <c r="E12" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="F12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H12" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="F12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="I12" s="1" t="s">
         <v>90</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="J12" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="K12" s="1" t="s">
         <v>92</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="L12" s="3" t="s">
         <v>93</v>
       </c>
-      <c r="L12" s="3" t="s">
+      <c r="M12" s="1" t="s">
         <v>94</v>
       </c>
-      <c r="M12" s="1" t="s">
+      <c r="N12" s="1" t="s">
         <v>95</v>
-      </c>
-      <c r="N12" s="1" t="s">
-        <v>96</v>
       </c>
     </row>
     <row r="13" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="B13" s="1" t="s">
         <v>148</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>149</v>
       </c>
       <c r="C13" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Thurmon Lockhart</v>
       </c>
       <c r="D13" s="1" t="s">
+        <v>149</v>
+      </c>
+      <c r="E13" s="1" t="s">
         <v>150</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>151</v>
       </c>
       <c r="F13" s="1" t="s">
         <v>28</v>
@@ -2321,33 +2321,33 @@
         <v>28</v>
       </c>
       <c r="H13" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="I13" s="1" t="s">
         <v>152</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="J13" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="K13" s="1" t="s">
         <v>154</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="L13" s="3" t="s">
         <v>155</v>
       </c>
-      <c r="L13" s="3" t="s">
+      <c r="M13" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="M13" s="1" t="s">
+      <c r="N13" s="1" t="s">
         <v>157</v>
-      </c>
-      <c r="N13" s="1" t="s">
-        <v>158</v>
       </c>
     </row>
     <row r="14" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B14" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>67</v>
       </c>
       <c r="C14" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2357,42 +2357,42 @@
         <v>38</v>
       </c>
       <c r="E14" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="F14" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="1" t="s">
+      <c r="G14" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H14" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="G14" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H14" s="3" t="s">
+      <c r="I14" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="I14" s="1" t="s">
+      <c r="J14" s="1" t="s">
         <v>71</v>
       </c>
-      <c r="J14" s="1" t="s">
+      <c r="K14" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="K14" s="1" t="s">
+      <c r="L14" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="L14" s="3" t="s">
+      <c r="M14" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="M14" s="1" t="s">
+      <c r="N14" s="1" t="s">
         <v>75</v>
-      </c>
-      <c r="N14" s="1" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="15" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B15" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="B15" s="1" t="s">
-        <v>129</v>
       </c>
       <c r="C15" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2402,7 +2402,7 @@
         <v>38</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F15" s="1" t="s">
         <v>18</v>
@@ -2411,33 +2411,33 @@
         <v>18</v>
       </c>
       <c r="H15" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="I15" s="1" t="s">
         <v>131</v>
       </c>
-      <c r="I15" s="1" t="s">
+      <c r="J15" s="1" t="s">
         <v>132</v>
       </c>
-      <c r="J15" s="1" t="s">
+      <c r="K15" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="K15" s="1" t="s">
+      <c r="L15" s="3" t="s">
         <v>134</v>
       </c>
-      <c r="L15" s="3" t="s">
+      <c r="M15" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="M15" s="1" t="s">
+      <c r="N15" s="1" t="s">
         <v>136</v>
-      </c>
-      <c r="N15" s="1" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="16" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
+        <v>178</v>
+      </c>
+      <c r="B16" s="1" t="s">
         <v>179</v>
-      </c>
-      <c r="B16" s="1" t="s">
-        <v>180</v>
       </c>
       <c r="C16" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2447,34 +2447,34 @@
         <v>38</v>
       </c>
       <c r="E16" s="1" t="s">
+        <v>180</v>
+      </c>
+      <c r="F16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G16" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H16" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="F16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G16" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="I16" s="1" t="s">
         <v>182</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="J16" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="K16" s="1" t="s">
         <v>184</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="L16" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="L16" s="3" t="s">
+      <c r="M16" s="1" t="s">
         <v>186</v>
       </c>
-      <c r="M16" s="1" t="s">
+      <c r="N16" s="1" t="s">
         <v>187</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="17" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
@@ -2521,10 +2521,10 @@
     </row>
     <row r="18" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
+        <v>208</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>209</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>210</v>
       </c>
       <c r="C18" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2534,7 +2534,7 @@
         <v>38</v>
       </c>
       <c r="E18" s="1" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="F18" s="1" t="s">
         <v>18</v>
@@ -2543,43 +2543,43 @@
         <v>18</v>
       </c>
       <c r="H18" s="3" t="s">
+        <v>211</v>
+      </c>
+      <c r="I18" s="1" t="s">
         <v>212</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="J18" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="J18" s="1" t="s">
+      <c r="K18" s="1" t="s">
         <v>214</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="L18" s="3" t="s">
         <v>215</v>
       </c>
-      <c r="L18" s="3" t="s">
+      <c r="M18" s="1" t="s">
         <v>216</v>
       </c>
-      <c r="M18" s="1" t="s">
+      <c r="N18" s="1" t="s">
         <v>217</v>
-      </c>
-      <c r="N18" s="1" t="s">
-        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="B19" s="1" t="s">
         <v>138</v>
-      </c>
-      <c r="B19" s="1" t="s">
-        <v>139</v>
       </c>
       <c r="C19" s="1" t="str">
         <f t="shared" si="0"/>
         <v>Thomas Sugar</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="E19" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="F19" s="1" t="s">
         <v>39</v>
@@ -2588,33 +2588,33 @@
         <v>39</v>
       </c>
       <c r="H19" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="I19" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="J19" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="K19" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="L19" s="3" t="s">
         <v>144</v>
       </c>
-      <c r="L19" s="3" t="s">
+      <c r="M19" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="M19" s="1" t="s">
+      <c r="N19" s="1" t="s">
         <v>146</v>
-      </c>
-      <c r="N19" s="1" t="s">
-        <v>147</v>
       </c>
     </row>
     <row r="20" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B20" s="1" t="s">
         <v>169</v>
-      </c>
-      <c r="B20" s="1" t="s">
-        <v>170</v>
       </c>
       <c r="C20" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2624,7 +2624,7 @@
         <v>38</v>
       </c>
       <c r="E20" s="1" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="F20" s="1" t="s">
         <v>18</v>
@@ -2633,33 +2633,33 @@
         <v>18</v>
       </c>
       <c r="H20" s="3" t="s">
+        <v>171</v>
+      </c>
+      <c r="I20" s="1" t="s">
         <v>172</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="J20" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="K20" s="1" t="s">
         <v>174</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="L20" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="L20" s="3" t="s">
+      <c r="M20" s="1" t="s">
         <v>176</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="N20" s="1" t="s">
         <v>177</v>
-      </c>
-      <c r="N20" s="1" t="s">
-        <v>178</v>
       </c>
     </row>
     <row r="21" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
+        <v>218</v>
+      </c>
+      <c r="B21" s="1" t="s">
         <v>219</v>
-      </c>
-      <c r="B21" s="1" t="s">
-        <v>220</v>
       </c>
       <c r="C21" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2669,42 +2669,42 @@
         <v>38</v>
       </c>
       <c r="E21" s="1" t="s">
+        <v>220</v>
+      </c>
+      <c r="F21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="G21" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="H21" s="3" t="s">
+        <v>239</v>
+      </c>
+      <c r="I21" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="F21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="G21" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H21" s="3" t="s">
-        <v>240</v>
-      </c>
-      <c r="I21" s="1" t="s">
+      <c r="J21" s="1" t="s">
         <v>222</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="K21" s="1" t="s">
         <v>223</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="L21" s="3" t="s">
         <v>224</v>
       </c>
-      <c r="L21" s="3" t="s">
+      <c r="M21" s="1" t="s">
         <v>225</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="N21" s="1" t="s">
         <v>226</v>
-      </c>
-      <c r="N21" s="1" t="s">
-        <v>227</v>
       </c>
     </row>
     <row r="22" spans="1:14" ht="25.5" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B22" s="1" t="s">
         <v>159</v>
-      </c>
-      <c r="B22" s="1" t="s">
-        <v>160</v>
       </c>
       <c r="C22" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2714,7 +2714,7 @@
         <v>38</v>
       </c>
       <c r="E22" s="1" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="F22" s="1" t="s">
         <v>39</v>
@@ -2723,33 +2723,33 @@
         <v>39</v>
       </c>
       <c r="H22" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="I22" s="1" t="s">
         <v>162</v>
       </c>
-      <c r="I22" s="1" t="s">
+      <c r="J22" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="J22" s="1" t="s">
+      <c r="K22" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="K22" s="1" t="s">
+      <c r="L22" s="3" t="s">
         <v>165</v>
       </c>
-      <c r="L22" s="3" t="s">
+      <c r="M22" s="1" t="s">
         <v>166</v>
       </c>
-      <c r="M22" s="1" t="s">
+      <c r="N22" s="1" t="s">
         <v>167</v>
-      </c>
-      <c r="N22" s="1" t="s">
-        <v>168</v>
       </c>
     </row>
     <row r="23" spans="1:14" ht="38.25" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B23" s="1" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="C23" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2759,7 +2759,7 @@
         <v>38</v>
       </c>
       <c r="E23" s="1" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="F23" s="1" t="s">
         <v>18</v>
@@ -2768,33 +2768,33 @@
         <v>18</v>
       </c>
       <c r="H23" s="3" t="s">
+        <v>201</v>
+      </c>
+      <c r="I23" s="1" t="s">
         <v>202</v>
       </c>
-      <c r="I23" s="1" t="s">
+      <c r="J23" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="J23" s="1" t="s">
+      <c r="K23" s="1" t="s">
         <v>204</v>
       </c>
-      <c r="K23" s="1" t="s">
+      <c r="L23" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="L23" s="3" t="s">
+      <c r="M23" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="M23" s="1" t="s">
+      <c r="N23" s="1" t="s">
         <v>207</v>
-      </c>
-      <c r="N23" s="1" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
+        <v>240</v>
+      </c>
+      <c r="B24" s="1" t="s">
         <v>241</v>
-      </c>
-      <c r="B24" s="1" t="s">
-        <v>242</v>
       </c>
       <c r="C24" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2804,7 +2804,7 @@
         <v>16</v>
       </c>
       <c r="E24" s="1" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="F24" s="1" t="s">
         <v>39</v>
@@ -2813,33 +2813,33 @@
         <v>39</v>
       </c>
       <c r="H24" s="3" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="I24" s="1" t="s">
+        <v>141</v>
+      </c>
+      <c r="J24" s="1" t="s">
         <v>142</v>
       </c>
-      <c r="J24" s="1" t="s">
+      <c r="K24" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="K24" s="1" t="s">
-        <v>144</v>
-      </c>
       <c r="L24" s="4" t="s">
+        <v>243</v>
+      </c>
+      <c r="M24" s="1" t="s">
         <v>244</v>
       </c>
-      <c r="M24" s="1" t="s">
+      <c r="N24" s="1" t="s">
         <v>245</v>
-      </c>
-      <c r="N24" s="1" t="s">
-        <v>246</v>
       </c>
     </row>
     <row r="25" spans="1:14" ht="51" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
+        <v>247</v>
+      </c>
+      <c r="B25" s="1" t="s">
         <v>248</v>
-      </c>
-      <c r="B25" s="1" t="s">
-        <v>249</v>
       </c>
       <c r="C25" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2849,7 +2849,7 @@
         <v>38</v>
       </c>
       <c r="E25" s="1" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="F25" s="1" t="s">
         <v>39</v>
@@ -2858,30 +2858,30 @@
         <v>39</v>
       </c>
       <c r="H25" s="3" t="s">
+        <v>250</v>
+      </c>
+      <c r="I25" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="I25" s="1" t="s">
+      <c r="J25" s="1" t="s">
         <v>252</v>
       </c>
-      <c r="J25" s="1" t="s">
+      <c r="L25" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="L25" s="3" t="s">
+      <c r="M25" s="1" t="s">
         <v>254</v>
       </c>
-      <c r="M25" s="1" t="s">
-        <v>255</v>
-      </c>
       <c r="N25" s="1" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26" spans="1:14" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A26" s="1" t="s">
+        <v>255</v>
+      </c>
+      <c r="B26" s="1" t="s">
         <v>256</v>
-      </c>
-      <c r="B26" s="1" t="s">
-        <v>257</v>
       </c>
       <c r="C26" s="1" t="str">
         <f t="shared" si="0"/>
@@ -2891,7 +2891,7 @@
         <v>38</v>
       </c>
       <c r="E26" s="1" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="F26" s="1" t="s">
         <v>39</v>
@@ -2900,19 +2900,19 @@
         <v>39</v>
       </c>
       <c r="H26" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="I26" s="5" t="s">
         <v>259</v>
       </c>
-      <c r="I26" s="5" t="s">
+      <c r="J26" s="1" t="s">
         <v>260</v>
       </c>
-      <c r="J26" s="1" t="s">
+      <c r="L26" s="3" t="s">
         <v>261</v>
       </c>
-      <c r="L26" s="3" t="s">
+      <c r="M26" s="1" t="s">
         <v>262</v>
-      </c>
-      <c r="M26" s="1" t="s">
-        <v>263</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added nancy and re-rendered images
</commit_message>
<xml_diff>
--- a/_data/faculty.xlsx
+++ b/_data/faculty.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="346" uniqueCount="277">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="288">
   <si>
     <t xml:space="preserve">first_name</t>
   </si>
@@ -851,6 +851,39 @@
   </si>
   <si>
     <t xml:space="preserve">ZheXu.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nancy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cooke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nancy Cooke</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ncooke@asu.edu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Study the characteristics of human-centered AI and Robotic teammates; develop metrics and measures to evaluate human-AI-robot teaming effectiveness; address AI/robot-related ethical issues.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Human-Robot,Design,Dynamics,AI-and-learning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Center for Human, Artificial Intelligence, and Robot Teaming</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://globalsecurity.asu.edu/expertise/human-artificial-intelligence-and-robot-teaming/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">We take a multidisciplinary approach to develop and evaluate effective human-AI-robot teams, as well as address related legal and ethical issues through human-in-the-loop studies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ncooke.png</t>
+  </si>
+  <si>
+    <t xml:space="preserve">asu-ghost-lab.jpg</t>
   </si>
 </sst>
 </file>
@@ -981,7 +1014,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1019,6 +1052,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1100,10 +1141,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:AMJ27"/>
+  <dimension ref="A1:AMJ28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A5" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F25" activeCellId="0" sqref="F25"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="L20" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="O28" activeCellId="0" sqref="O28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1484375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1114,7 +1155,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="30.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="23.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="38.29"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="16.89"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="2" width="75"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="9" style="1" width="40.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="2" width="80.57"/>
@@ -3326,10 +3367,56 @@
       <c r="AMI27" s="9"/>
       <c r="AMJ27" s="9"/>
     </row>
+    <row r="28" customFormat="false" ht="20.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="1" t="s">
+        <v>277</v>
+      </c>
+      <c r="B28" s="1" t="s">
+        <v>278</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>279</v>
+      </c>
+      <c r="D28" s="1" t="s">
+        <v>106</v>
+      </c>
+      <c r="E28" s="10" t="s">
+        <v>280</v>
+      </c>
+      <c r="F28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="G28" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="H28" s="2" t="s">
+        <v>281</v>
+      </c>
+      <c r="I28" s="1" t="s">
+        <v>282</v>
+      </c>
+      <c r="J28" s="1" t="s">
+        <v>283</v>
+      </c>
+      <c r="K28" s="11" t="s">
+        <v>284</v>
+      </c>
+      <c r="L28" s="2" t="s">
+        <v>285</v>
+      </c>
+      <c r="M28" s="1" t="s">
+        <v>286</v>
+      </c>
+      <c r="N28" s="1" t="s">
+        <v>287</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" display="danaukes@asu.edu"/>
     <hyperlink ref="K27" r:id="rId2" display="https://sites.google.com/site/zhexudavid00710"/>
+    <hyperlink ref="E28" r:id="rId3" display="ncooke@asu.edu"/>
+    <hyperlink ref="K28" r:id="rId4" display="https://globalsecurity.asu.edu/expertise/human-artificial-intelligence-and-robot-teaming/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>